<commit_message>
UPDATED : input rank by number
</commit_message>
<xml_diff>
--- a/tekken7_draw_complete.xlsx
+++ b/tekken7_draw_complete.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G36"/>
+  <dimension ref="A1:G49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -472,28 +472,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>NO10</t>
+          <t xml:space="preserve">삐깃 </t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>XU76</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>True Tekken God</t>
-        </is>
+          <t>QA13</t>
+        </is>
+      </c>
+      <c r="D2" t="n">
+        <v>31</v>
       </c>
       <c r="E2" t="n">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="F2" t="n">
-        <v>15.3</v>
+        <v>18</v>
       </c>
       <c r="G2" t="inlineStr">
         <is>
@@ -503,28 +501,26 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>DQ52</t>
+          <t xml:space="preserve">보이조지 </t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>RL11</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>1th</t>
-        </is>
+          <t>SL19</t>
+        </is>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
       </c>
       <c r="E3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="F3" t="n">
-        <v>15.3</v>
+        <v>18</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -534,28 +530,26 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>13</v>
+        <v>1</v>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>JZ31</t>
+          <t xml:space="preserve">킹넘약 </t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>KT54</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>Vindicator</t>
-        </is>
+          <t>BY96</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>18</v>
       </c>
       <c r="E4" t="n">
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="F4" t="n">
-        <v>15.3</v>
+        <v>18</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -565,28 +559,26 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>34</v>
+        <v>44</v>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>UX70</t>
+          <t xml:space="preserve">커여운웰시코기 </t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>AO90</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>Tekken God</t>
-        </is>
+          <t>NQ96</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>31</v>
       </c>
       <c r="E5" t="n">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F5" t="n">
-        <v>15.7</v>
+        <v>18.7</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -596,28 +588,26 @@
     </row>
     <row r="6">
       <c r="A6" t="n">
-        <v>2</v>
+        <v>41</v>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>DX48</t>
+          <t xml:space="preserve">먼지마냥 </t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>CA73</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>2th</t>
-        </is>
+          <t>SQ75</t>
+        </is>
+      </c>
+      <c r="D6" t="n">
+        <v>6</v>
       </c>
       <c r="E6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F6" t="n">
-        <v>15.7</v>
+        <v>18.7</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -627,28 +617,26 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>14</v>
+        <v>42</v>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>WE51</t>
+          <t xml:space="preserve">몽스터 </t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>LQ12</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>Juggernaut</t>
-        </is>
+          <t>TX50</t>
+        </is>
+      </c>
+      <c r="D7" t="n">
+        <v>19</v>
       </c>
       <c r="E7" t="n">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F7" t="n">
-        <v>15.7</v>
+        <v>18.7</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -658,28 +646,26 @@
     </row>
     <row r="8">
       <c r="A8" t="n">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>SZ50</t>
+          <t xml:space="preserve">9pu </t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>DZ40</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>Tekken King</t>
-        </is>
+          <t>DB50</t>
+        </is>
+      </c>
+      <c r="D8" t="n">
+        <v>30</v>
       </c>
       <c r="E8" t="n">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F8" t="n">
-        <v>16</v>
+        <v>19.3</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -689,28 +675,26 @@
     </row>
     <row r="9">
       <c r="A9" t="n">
-        <v>3</v>
+        <v>18</v>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>TB22</t>
+          <t xml:space="preserve">미친쓰레기 </t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AF91</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>3th</t>
-        </is>
+          <t>RL31</t>
+        </is>
+      </c>
+      <c r="D9" t="n">
+        <v>9</v>
       </c>
       <c r="E9" t="n">
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="F9" t="n">
-        <v>16</v>
+        <v>19.3</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -720,28 +704,26 @@
     </row>
     <row r="10">
       <c r="A10" t="n">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>FK13</t>
+          <t xml:space="preserve">밥스터 </t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>CP20</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>Usurper</t>
-        </is>
+          <t>PE35</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>19</v>
       </c>
       <c r="E10" t="n">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="F10" t="n">
-        <v>16</v>
+        <v>19.3</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -751,28 +733,26 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>YU85</t>
+          <t xml:space="preserve">지릉 </t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LF99</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>Emperor</t>
-        </is>
+          <t>UP33</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>29</v>
       </c>
       <c r="E11" t="n">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F11" t="n">
-        <v>16.3</v>
+        <v>19.3</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -782,28 +762,26 @@
     </row>
     <row r="12">
       <c r="A12" t="n">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>GJ48</t>
+          <t xml:space="preserve">같이있던가치 </t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>TY29</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>Initiate</t>
-        </is>
+          <t>DX83</t>
+        </is>
+      </c>
+      <c r="D12" t="n">
+        <v>9</v>
       </c>
       <c r="E12" t="n">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="F12" t="n">
-        <v>16.3</v>
+        <v>19.3</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -813,28 +791,26 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>16</v>
+        <v>37</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>GR15</t>
+          <t xml:space="preserve">XsWon </t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>XQ54</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>Vanquisher</t>
-        </is>
+          <t>VO17</t>
+        </is>
+      </c>
+      <c r="D13" t="n">
+        <v>20</v>
       </c>
       <c r="E13" t="n">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F13" t="n">
-        <v>16.3</v>
+        <v>19.3</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -844,28 +820,26 @@
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>31</v>
+        <v>6</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>TA25</t>
+          <t xml:space="preserve">JwaJuL </t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>KS52</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>Ryujin</t>
-        </is>
+          <t>FH89</t>
+        </is>
+      </c>
+      <c r="D14" t="n">
+        <v>28</v>
       </c>
       <c r="E14" t="n">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F14" t="n">
-        <v>16.7</v>
+        <v>20</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -875,28 +849,26 @@
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>YS60</t>
+          <t xml:space="preserve">shy_Bugi </t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>BY15</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>Mentor</t>
-        </is>
+          <t>LK33</t>
+        </is>
+      </c>
+      <c r="D15" t="n">
+        <v>12</v>
       </c>
       <c r="E15" t="n">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="F15" t="n">
-        <v>16.7</v>
+        <v>20</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -906,28 +878,26 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>17</v>
+        <v>8</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>CO31</t>
+          <t xml:space="preserve">욱코 </t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>UW73</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>Destroyer</t>
-        </is>
+          <t>PR79</t>
+        </is>
+      </c>
+      <c r="D16" t="n">
+        <v>20</v>
       </c>
       <c r="E16" t="n">
-        <v>16</v>
+        <v>20</v>
       </c>
       <c r="F16" t="n">
-        <v>16.7</v>
+        <v>20</v>
       </c>
       <c r="G16" t="inlineStr">
         <is>
@@ -937,28 +907,26 @@
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>PP39</t>
+          <t xml:space="preserve">qwertyop </t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>CC90</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>Yaksa</t>
-        </is>
+          <t>ZE58</t>
+        </is>
+      </c>
+      <c r="D17" t="n">
+        <v>28</v>
       </c>
       <c r="E17" t="n">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F17" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G17" t="inlineStr">
         <is>
@@ -968,28 +936,26 @@
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>6</v>
+        <v>14</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>FP33</t>
+          <t xml:space="preserve">감자탕 </t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>DX48</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>Expert</t>
-        </is>
+          <t>AB86</t>
+        </is>
+      </c>
+      <c r="D18" t="n">
+        <v>12</v>
       </c>
       <c r="E18" t="n">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F18" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G18" t="inlineStr">
         <is>
@@ -999,28 +965,26 @@
     </row>
     <row r="19">
       <c r="A19" t="n">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>MF16</t>
+          <t xml:space="preserve">김콧털 </t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>HA75</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>Savior</t>
-        </is>
+          <t>SH53</t>
+        </is>
+      </c>
+      <c r="D19" t="n">
+        <v>20</v>
       </c>
       <c r="E19" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="F19" t="n">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="G19" t="inlineStr">
         <is>
@@ -1030,28 +994,26 @@
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>TX71</t>
+          <t xml:space="preserve">윌프 </t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>ML62</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>Raijin</t>
-        </is>
+          <t>LM82</t>
+        </is>
+      </c>
+      <c r="D20" t="n">
+        <v>28</v>
       </c>
       <c r="E20" t="n">
         <v>28</v>
       </c>
       <c r="F20" t="n">
-        <v>17.3</v>
+        <v>20.3</v>
       </c>
       <c r="G20" t="inlineStr">
         <is>
@@ -1061,28 +1023,26 @@
     </row>
     <row r="21">
       <c r="A21" t="n">
-        <v>7</v>
+        <v>46</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>IQ14</t>
+          <t xml:space="preserve">Elma1219 </t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>ZJ90</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>Grand Master</t>
-        </is>
+          <t>OM50</t>
+        </is>
+      </c>
+      <c r="D21" t="n">
+        <v>13</v>
       </c>
       <c r="E21" t="n">
-        <v>6</v>
+        <v>13</v>
       </c>
       <c r="F21" t="n">
-        <v>17.3</v>
+        <v>20.3</v>
       </c>
       <c r="G21" t="inlineStr">
         <is>
@@ -1092,28 +1052,26 @@
     </row>
     <row r="22">
       <c r="A22" t="n">
-        <v>19</v>
+        <v>3</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>SE95</t>
+          <t xml:space="preserve">여름싫어 </t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>BM39</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>Overlord</t>
-        </is>
+          <t>OJ51</t>
+        </is>
+      </c>
+      <c r="D22" t="n">
+        <v>20</v>
       </c>
       <c r="E22" t="n">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F22" t="n">
-        <v>17.3</v>
+        <v>20.3</v>
       </c>
       <c r="G22" t="inlineStr">
         <is>
@@ -1123,28 +1081,26 @@
     </row>
     <row r="23">
       <c r="A23" t="n">
+        <v>29</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t xml:space="preserve">하지마~ </t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>NQ67</t>
+        </is>
+      </c>
+      <c r="D23" t="n">
         <v>28</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>RR34</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>BK40</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>Fujin</t>
-        </is>
-      </c>
       <c r="E23" t="n">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F23" t="n">
-        <v>17.7</v>
+        <v>20.7</v>
       </c>
       <c r="G23" t="inlineStr">
         <is>
@@ -1154,28 +1110,26 @@
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>8</v>
+        <v>38</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>DW91</t>
+          <t xml:space="preserve">츠미시요 </t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>XW54</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Brawler</t>
-        </is>
+          <t>GT25</t>
+        </is>
+      </c>
+      <c r="D24" t="n">
+        <v>13</v>
       </c>
       <c r="E24" t="n">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F24" t="n">
-        <v>17.7</v>
+        <v>20.7</v>
       </c>
       <c r="G24" t="inlineStr">
         <is>
@@ -1185,28 +1139,26 @@
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>SH52</t>
+          <t xml:space="preserve">월평 </t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>UA74</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Genbu</t>
-        </is>
+          <t>SF53</t>
+        </is>
+      </c>
+      <c r="D25" t="n">
+        <v>21</v>
       </c>
       <c r="E25" t="n">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F25" t="n">
-        <v>17.7</v>
+        <v>20.7</v>
       </c>
       <c r="G25" t="inlineStr">
         <is>
@@ -1216,28 +1168,26 @@
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>27</v>
+        <v>43</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>BD60</t>
+          <t xml:space="preserve">우매봉탈출불가 </t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>TJ36</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Eternal Ruler</t>
-        </is>
+          <t>YP39</t>
+        </is>
+      </c>
+      <c r="D26" t="n">
+        <v>28</v>
       </c>
       <c r="E26" t="n">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="F26" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G26" t="inlineStr">
         <is>
@@ -1247,28 +1197,26 @@
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>PK66</t>
+          <t xml:space="preserve">피고티 </t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>IY17</t>
-        </is>
-      </c>
-      <c r="D27" t="inlineStr">
-        <is>
-          <t>Marauder</t>
-        </is>
+          <t>ZH48</t>
+        </is>
+      </c>
+      <c r="D27" t="n">
+        <v>13</v>
       </c>
       <c r="E27" t="n">
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="F27" t="n">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="G27" t="inlineStr">
         <is>
@@ -1278,28 +1226,26 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
+        <v>24</v>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t xml:space="preserve">FreezingBlue </t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>IO94</t>
+        </is>
+      </c>
+      <c r="D28" t="n">
+        <v>22</v>
+      </c>
+      <c r="E28" t="n">
+        <v>22</v>
+      </c>
+      <c r="F28" t="n">
         <v>21</v>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>HX15</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>SB88</t>
-        </is>
-      </c>
-      <c r="D28" t="inlineStr">
-        <is>
-          <t>Byakko</t>
-        </is>
-      </c>
-      <c r="E28" t="n">
-        <v>20</v>
-      </c>
-      <c r="F28" t="n">
-        <v>18</v>
       </c>
       <c r="G28" t="inlineStr">
         <is>
@@ -1309,28 +1255,26 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>CP66</t>
+          <t xml:space="preserve">Ryyoon </t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>IT13</t>
-        </is>
-      </c>
-      <c r="D29" t="inlineStr">
-        <is>
-          <t>Divine Ruler</t>
-        </is>
+          <t>KO61</t>
+        </is>
+      </c>
+      <c r="D29" t="n">
+        <v>27</v>
       </c>
       <c r="E29" t="n">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F29" t="n">
-        <v>18.3</v>
+        <v>21</v>
       </c>
       <c r="G29" t="inlineStr">
         <is>
@@ -1340,28 +1284,26 @@
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>QX62</t>
+          <t xml:space="preserve">조온순 </t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>YB95</t>
-        </is>
-      </c>
-      <c r="D30" t="inlineStr">
-        <is>
-          <t>Fighter</t>
-        </is>
+          <t>ZU70</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
+        <v>14</v>
       </c>
       <c r="E30" t="n">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="F30" t="n">
-        <v>18.3</v>
+        <v>21</v>
       </c>
       <c r="G30" t="inlineStr">
         <is>
@@ -1371,28 +1313,26 @@
     </row>
     <row r="31">
       <c r="A31" t="n">
+        <v>23</v>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t xml:space="preserve">작은새 </t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>JD14</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
         <v>22</v>
       </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>SC30</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>XK90</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Seiryu</t>
-        </is>
-      </c>
       <c r="E31" t="n">
+        <v>22</v>
+      </c>
+      <c r="F31" t="n">
         <v>21</v>
-      </c>
-      <c r="F31" t="n">
-        <v>18.3</v>
       </c>
       <c r="G31" t="inlineStr">
         <is>
@@ -1402,28 +1342,26 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>QU35</t>
+          <t xml:space="preserve">Ako </t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>QQ91</t>
-        </is>
-      </c>
-      <c r="D32" t="inlineStr">
-        <is>
-          <t>Revered Ruler</t>
-        </is>
+          <t>QL15</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
+        <v>26</v>
       </c>
       <c r="E32" t="n">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F32" t="n">
-        <v>18.7</v>
+        <v>21.3</v>
       </c>
       <c r="G32" t="inlineStr">
         <is>
@@ -1433,28 +1371,26 @@
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>11</v>
+        <v>17</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>JR47</t>
+          <t xml:space="preserve">sooooooo </t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>FZ49</t>
-        </is>
-      </c>
-      <c r="D33" t="inlineStr">
-        <is>
-          <t>Vanguard</t>
-        </is>
+          <t>SE62</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
+        <v>15</v>
       </c>
       <c r="E33" t="n">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="F33" t="n">
-        <v>18.7</v>
+        <v>21.3</v>
       </c>
       <c r="G33" t="inlineStr">
         <is>
@@ -1464,28 +1400,26 @@
     </row>
     <row r="34">
       <c r="A34" t="n">
+        <v>40</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t xml:space="preserve">우일신 </t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>GV50</t>
+        </is>
+      </c>
+      <c r="D34" t="n">
         <v>23</v>
       </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>CR96</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>VP79</t>
-        </is>
-      </c>
-      <c r="D34" t="inlineStr">
-        <is>
-          <t>Suzaku</t>
-        </is>
-      </c>
       <c r="E34" t="n">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="F34" t="n">
-        <v>18.7</v>
+        <v>21.3</v>
       </c>
       <c r="G34" t="inlineStr">
         <is>
@@ -1495,28 +1429,26 @@
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
-          <t>QW60</t>
+          <t xml:space="preserve">딱지충 </t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>PD89</t>
-        </is>
-      </c>
-      <c r="D35" t="inlineStr">
-        <is>
-          <t>Mighty Ruler</t>
-        </is>
+          <t>JD73</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
+        <v>26</v>
       </c>
       <c r="E35" t="n">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F35" t="n">
-        <v>17</v>
+        <v>21.7</v>
       </c>
       <c r="G35" t="inlineStr">
         <is>
@@ -1526,32 +1458,407 @@
     </row>
     <row r="36">
       <c r="A36" t="n">
+        <v>32</v>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Hyoka </t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>AZ70</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
+        <v>16</v>
+      </c>
+      <c r="E36" t="n">
+        <v>16</v>
+      </c>
+      <c r="F36" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>11조</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>35</v>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t xml:space="preserve">나즈막히 </t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>MM61</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
+        <v>23</v>
+      </c>
+      <c r="E37" t="n">
+        <v>23</v>
+      </c>
+      <c r="F37" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>11조</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>2</v>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t xml:space="preserve">백산수 </t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>FV34</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
+        <v>25</v>
+      </c>
+      <c r="E38" t="n">
+        <v>25</v>
+      </c>
+      <c r="F38" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>12조</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>22</v>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t xml:space="preserve">ddongco </t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>LB32</t>
+        </is>
+      </c>
+      <c r="D39" t="n">
+        <v>16</v>
+      </c>
+      <c r="E39" t="n">
+        <v>16</v>
+      </c>
+      <c r="F39" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>12조</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>16</v>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t xml:space="preserve">공오 </t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>XX88</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
+        <v>23</v>
+      </c>
+      <c r="E40" t="n">
+        <v>23</v>
+      </c>
+      <c r="F40" t="n">
+        <v>21.3</v>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>12조</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>45</v>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t xml:space="preserve">마요바요 </t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>GE26</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
+        <v>25</v>
+      </c>
+      <c r="E41" t="n">
+        <v>25</v>
+      </c>
+      <c r="F41" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>13조</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>13</v>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t xml:space="preserve">미겔잼추털 </t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>PB96</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
+        <v>16</v>
+      </c>
+      <c r="E42" t="n">
+        <v>16</v>
+      </c>
+      <c r="F42" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>13조</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="n">
+        <v>47</v>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t xml:space="preserve">돼지햄 </t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>XV62</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
+        <v>24</v>
+      </c>
+      <c r="E43" t="n">
+        <v>24</v>
+      </c>
+      <c r="F43" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>13조</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="n">
+        <v>7</v>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t xml:space="preserve">RAK </t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>NQ83</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
+        <v>24</v>
+      </c>
+      <c r="E44" t="n">
+        <v>24</v>
+      </c>
+      <c r="F44" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>14조</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="n">
         <v>12</v>
       </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>NU65</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>GL73</t>
-        </is>
-      </c>
-      <c r="D36" t="inlineStr">
-        <is>
-          <t>Warrior</t>
-        </is>
-      </c>
-      <c r="E36" t="n">
-        <v>11</v>
-      </c>
-      <c r="F36" t="n">
+      <c r="B45" t="inlineStr">
+        <is>
+          <t xml:space="preserve">막산다 </t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>DQ71</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
         <v>17</v>
       </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>11조</t>
+      <c r="E45" t="n">
+        <v>17</v>
+      </c>
+      <c r="F45" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>14조</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="n">
+        <v>36</v>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t xml:space="preserve">레인보우 </t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>TD64</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
+        <v>24</v>
+      </c>
+      <c r="E46" t="n">
+        <v>24</v>
+      </c>
+      <c r="F46" t="n">
+        <v>21.7</v>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>14조</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="n">
+        <v>27</v>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t xml:space="preserve">커포포링 </t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>RD39</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
+        <v>24</v>
+      </c>
+      <c r="E47" t="n">
+        <v>24</v>
+      </c>
+      <c r="F47" t="n">
+        <v>22</v>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>15조</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="n">
+        <v>48</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t xml:space="preserve">하다솜 </t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>PT78</t>
+        </is>
+      </c>
+      <c r="D48" t="n">
+        <v>18</v>
+      </c>
+      <c r="E48" t="n">
+        <v>18</v>
+      </c>
+      <c r="F48" t="n">
+        <v>22</v>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>15조</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="n">
+        <v>28</v>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t xml:space="preserve">catsoul </t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>DM19</t>
+        </is>
+      </c>
+      <c r="D49" t="n">
+        <v>24</v>
+      </c>
+      <c r="E49" t="n">
+        <v>24</v>
+      </c>
+      <c r="F49" t="n">
+        <v>22</v>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>15조</t>
         </is>
       </c>
     </row>

</xml_diff>